<commit_message>
updated user profile testcases
</commit_message>
<xml_diff>
--- a/selenium/com.MyCAlerts.POC/ApplicationTestData/AppData.xlsx
+++ b/selenium/com.MyCAlerts.POC/ApplicationTestData/AppData.xlsx
@@ -11,12 +11,12 @@
     <sheet name="TC02_UserProfile" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>admin@cgi.com</t>
   </si>
@@ -531,27 +531,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="9" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -586,15 +586,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
+      <c r="C2" s="1" t="str">
+        <f ca="1">CONCATENATE(A2,L2)</f>
+        <v>venkat99.637505614626</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -619,14 +620,18 @@
       </c>
       <c r="K2" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="L2">
+        <f ca="1">RAND()*100</f>
+        <v>99.637505614625994</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="K2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4" display="venkat@cgi.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the valid email address
</commit_message>
<xml_diff>
--- a/selenium/com.MyCAlerts.POC/ApplicationTestData/AppData.xlsx
+++ b/selenium/com.MyCAlerts.POC/ApplicationTestData/AppData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>admin@cgi.com</t>
   </si>
@@ -72,12 +72,6 @@
     <t>profile_ZipCode</t>
   </si>
   <si>
-    <t>mareedu</t>
-  </si>
-  <si>
-    <t>dada@123</t>
-  </si>
-  <si>
     <t>profile_PhNumber</t>
   </si>
   <si>
@@ -106,6 +100,15 @@
   </si>
   <si>
     <t>dada@1234</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>password@1</t>
   </si>
 </sst>
 </file>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,67 +574,67 @@
         <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="str">
         <f ca="1">CONCATENATE(A2,L2)</f>
-        <v>venkat99.637505614626</v>
+        <v>auto37.0607780579127</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>11111</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2">
-        <v>76502</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L2">
         <f ca="1">RAND()*100</f>
-        <v>99.637505614625994</v>
+        <v>37.060778057912692</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="K2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4" display="venkat@cgi.com"/>
+    <hyperlink ref="K2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3" display="venkat@cgi.com"/>
+    <hyperlink ref="E2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>